<commit_message>
fixiing printing indiv and group fixing tax and vat
</commit_message>
<xml_diff>
--- a/ProjectX/wwwroot/Samplefile/manualproduction.xlsx
+++ b/ProjectX/wwwroot/Samplefile/manualproduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://copere961-my.sharepoint.com/personal/falreiz_cope-ts_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\it4\Source\Workspaces\Workspace\My Project\Project X\ProjectX - v5\ProjectX\wwwroot\Samplefile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D634D10-A800-4E4A-9790-1B0159CCD224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E658282F-A9F9-4B88-B69C-7B07E3DF1D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>REF#</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>worldwide</t>
+  </si>
+  <si>
+    <t>Country of residence</t>
+  </si>
+  <si>
+    <t>Deductible</t>
+  </si>
+  <si>
+    <t>Sports Activities</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -462,21 +477,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P2"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,14 +534,23 @@
       <c r="N1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -566,11 +590,22 @@
       <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5">
+      <c r="N2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="5">
         <v>130.19999999999999</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>